<commit_message>
web ui solution using playwright and TS and bug report
</commit_message>
<xml_diff>
--- a/Bugs/Bugs.xlsx
+++ b/Bugs/Bugs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mine\Bugs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F4A470-ACA7-4956-BB15-D1EBB603F3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1E4B5B-1BB6-4970-A420-89F9239ED9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,40 +24,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="2">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="1"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="2">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-    <bk>
-      <rc t="1" v="1"/>
-    </bk>
-  </valueMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Title</t>
   </si>
@@ -98,9 +66,6 @@
     <t>Error Message should appear indicating that user alreay exists</t>
   </si>
   <si>
-    <t xml:space="preserve">user registered succesfully </t>
-  </si>
-  <si>
     <t>unhandled exception should be handled and user friendly message should appear instead</t>
   </si>
   <si>
@@ -111,12 +76,6 @@
   </si>
   <si>
     <t xml:space="preserve">User gets unhandled exception with exceeds limits </t>
-  </si>
-  <si>
-    <t xml:space="preserve">After Investigation , this error appears when trying to login or register in Edge, Chrome or Firefox after login with invalid data multiple times.
-In each request , a header is sent (X-Tractive-Client) with the same value.
-The response for login or register requests as in screenshot doesn't have detailed information.
-</t>
   </si>
   <si>
     <t xml:space="preserve">Register user succesfully.
@@ -160,12 +119,41 @@
   <si>
     <t>Medium</t>
   </si>
+  <si>
+    <t xml:space="preserve">user registered succesfully and is redirected to Activation TrackID </t>
+  </si>
+  <si>
+    <t>wrongpassword.png</t>
+  </si>
+  <si>
+    <t>notregisteredemail.png</t>
+  </si>
+  <si>
+    <t>unhandle2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">response.png
+</t>
+  </si>
+  <si>
+    <t>Error message doesn’t provide any information on the problem and how to fix it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After Investigation , this error appears when trying to login or register in Edge, Chrome or Firefox after login with invalid data multiple times.
+In each request , a header is sent (X-Tractive-Client) with the same value.
+The response for login or register requests doesn't have detailed information.
+The error disappeared after a day.
+</t>
+  </si>
+  <si>
+    <t>Instead of unhandled exception , user should be provided with a clear message describe the issue and how to be able to access system again.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +164,14 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -204,10 +200,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -215,8 +212,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -236,75 +238,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>1</v>
-    <v>5</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-  <rel r:id="rId2"/>
-</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -572,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,13 +548,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -635,19 +568,22 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -655,19 +591,22 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -675,56 +614,60 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" t="e" vm="1">
-        <v>#VALUE!</v>
+      <c r="G5" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E7" s="2"/>
-      <c r="G7" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="G7" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -742,7 +685,13 @@
       <c r="E9" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{97AB031F-820B-477B-B7EF-90FD381CC8EC}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{F3341489-A2FA-4C11-90CC-67B14B6AD0CF}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{D08EA969-A516-42C0-89AA-F6586750DCF4}"/>
+    <hyperlink ref="G7" r:id="rId4" display="response.png" xr:uid="{EA912737-14E4-4730-A5E5-673485080CB8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>